<commit_message>
Storing only package name in recommended packages
</commit_message>
<xml_diff>
--- a/Feedback_File.xlsx
+++ b/Feedback_File.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,6 +521,26 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Universal Guide Masthead - US (Weekend Heavy-Up), Apps Store Masthead - US</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>First Screen Immersive Roadblock, First Screen Rotational Roadblock, Spotlight Row Roadblock</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>First Screen Immersive Roadblock</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>